<commit_message>
Update Statistics of Feedback Control.xlsx
</commit_message>
<xml_diff>
--- a/Statistics of Feedback Control.xlsx
+++ b/Statistics of Feedback Control.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ziditao/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ziditao/Library/CloudStorage/Box-Box/Documents/Research/CDC 2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC743FD9-3CFF-FC49-8262-1A6CABA31D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D34100-C719-B74A-821B-B728F1191733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{6B9ED702-0638-1D46-89D3-5AE95F6BE353}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>TO</t>
   </si>
@@ -50,164 +50,145 @@
     <t xml:space="preserve">Var of </t>
   </si>
   <si>
-    <t xml:space="preserve">Quartile of </t>
-  </si>
-  <si>
-    <t>0.331*</t>
-  </si>
-  <si>
-    <t>0.444*</t>
-  </si>
-  <si>
-    <t>46.45, 58.69, 93.76</t>
-  </si>
-  <si>
-    <t>88.98, 107.41, 155.34</t>
-  </si>
-  <si>
-    <t>61.65*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.90, 57.55, 90.38 </t>
-  </si>
-  <si>
-    <t>66.00*</t>
-  </si>
-  <si>
-    <t>85.95, 108.35, 153.47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">214.42, 233.89, 240.64 </t>
-  </si>
-  <si>
-    <t>109.23*</t>
-  </si>
-  <si>
-    <t>136.03, 155.82, 214.43</t>
-  </si>
-  <si>
-    <t>0.0337*</t>
-  </si>
-  <si>
-    <t>236.12*</t>
-  </si>
-  <si>
-    <t>214.82, 233.96, 239.63</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.0039* </t>
-  </si>
-  <si>
-    <t>129.48 136.14 155.40</t>
-  </si>
-  <si>
-    <t>74.68*</t>
-  </si>
-  <si>
-    <t>75.89, 91.20, 112.60</t>
-  </si>
-  <si>
-    <t>86.56, 107.78, 135.64</t>
-  </si>
-  <si>
-    <t>0.0429*</t>
-  </si>
-  <si>
-    <t>81.75*</t>
-  </si>
-  <si>
-    <t>82.98, 107.85, 119.93</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67.70, 77.56, 96.18 </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Quartile of  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Cambria Math"/>
-        <family val="1"/>
-      </rPr>
-      <t>J</t>
-    </r>
-  </si>
-  <si>
-    <t>66.51*</t>
-  </si>
-  <si>
-    <t>52.46, 66.79, 100.86</t>
-  </si>
-  <si>
-    <t>0.205*</t>
-  </si>
-  <si>
-    <t>0.0040*</t>
-  </si>
-  <si>
-    <t>50.13, 62.28, 94.41</t>
-  </si>
-  <si>
-    <t>95.22, 120.29, 161.32</t>
-  </si>
-  <si>
-    <t>100.62 119.32 149.43</t>
-  </si>
-  <si>
-    <t>75.07*</t>
-  </si>
-  <si>
-    <t>0.302*</t>
-  </si>
-  <si>
-    <t>201.67*</t>
-  </si>
-  <si>
-    <t>68.23*</t>
-  </si>
-  <si>
-    <t>0.0473*</t>
-  </si>
-  <si>
-    <t>71.62*</t>
-  </si>
-  <si>
-    <t>183.54, 199.96, 206.17</t>
-  </si>
-  <si>
-    <t>184.09, 199.69, 205.87</t>
-  </si>
-  <si>
-    <t>69.68, 79.98, 102.14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61.87, 70.58, 88.62 </t>
-  </si>
-  <si>
-    <t>106.97*</t>
-  </si>
-  <si>
-    <t>108.44, 140.94, 155.16</t>
-  </si>
-  <si>
-    <t>109.33, 141.83, 150.18</t>
-  </si>
-  <si>
-    <t>85.45, 108.16, 121.63</t>
-  </si>
-  <si>
-    <t>82.24, 114.06, 127.60</t>
-  </si>
-  <si>
-    <t>0.140*</t>
-  </si>
-  <si>
-    <t>0.0486*</t>
+    <t>Mean of J</t>
+  </si>
+  <si>
+    <t>40.46*</t>
+  </si>
+  <si>
+    <t>41,86</t>
+  </si>
+  <si>
+    <t>54.31*</t>
+  </si>
+  <si>
+    <t>28.33*</t>
+  </si>
+  <si>
+    <t>Paired T-test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean of </t>
+  </si>
+  <si>
+    <t>15.80*</t>
+  </si>
+  <si>
+    <t>Var of J</t>
+  </si>
+  <si>
+    <t>14.14*</t>
+  </si>
+  <si>
+    <t>14.17*</t>
+  </si>
+  <si>
+    <t>13.28*</t>
+  </si>
+  <si>
+    <t>1.70*</t>
+  </si>
+  <si>
+    <t>27.88*</t>
+  </si>
+  <si>
+    <t>80.08*</t>
+  </si>
+  <si>
+    <t>162.50*</t>
+  </si>
+  <si>
+    <t>107.83*</t>
+  </si>
+  <si>
+    <t>173.96*</t>
+  </si>
+  <si>
+    <t>92.19*</t>
+  </si>
+  <si>
+    <t>54.54*</t>
+  </si>
+  <si>
+    <t>18.14*</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>38.58*</t>
+  </si>
+  <si>
+    <t>188.95*</t>
+  </si>
+  <si>
+    <t>73.26*</t>
+  </si>
+  <si>
+    <t>5.01*</t>
+  </si>
+  <si>
+    <t>70.31*</t>
+  </si>
+  <si>
+    <t>73.69*</t>
+  </si>
+  <si>
+    <t>60.68*</t>
+  </si>
+  <si>
+    <t>53.43*</t>
+  </si>
+  <si>
+    <t>56.98*</t>
+  </si>
+  <si>
+    <t>83.23*</t>
+  </si>
+  <si>
+    <t>87.09*</t>
+  </si>
+  <si>
+    <t>110.21*</t>
+  </si>
+  <si>
+    <t>108.61*</t>
+  </si>
+  <si>
+    <t>92.43*</t>
+  </si>
+  <si>
+    <t>24.61*</t>
+  </si>
+  <si>
+    <t>10.55*</t>
+  </si>
+  <si>
+    <t>19.82*</t>
+  </si>
+  <si>
+    <t>28.73*</t>
+  </si>
+  <si>
+    <t>11.34*</t>
+  </si>
+  <si>
+    <t>3.69*</t>
+  </si>
+  <si>
+    <t>20.15*</t>
+  </si>
+  <si>
+    <t>3.04*</t>
+  </si>
+  <si>
+    <t>19.53*</t>
+  </si>
+  <si>
+    <t>4.24*</t>
   </si>
 </sst>
 </file>
@@ -244,11 +225,11 @@
     </font>
     <font>
       <b/>
-      <i/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Cambria Math"/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -333,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -358,6 +339,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -497,8 +502,8 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="238399" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -540,6 +545,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -579,7 +585,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -643,8 +649,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="378565" cy="236155"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -686,6 +692,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -725,7 +732,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -788,143 +795,53 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="178702" cy="187872"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="TextBox 6">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{693E145C-E650-345F-689D-D8BB55495237}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2813050" y="38100"/>
-              <a:ext cx="178702" cy="187872"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑱</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝒏</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1200" b="1"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="TextBox 6">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{693E145C-E650-345F-689D-D8BB55495237}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2813050" y="38100"/>
-              <a:ext cx="178702" cy="187872"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="1" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑱_𝒏</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1200" b="1"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <xdr:ext cx="65" cy="187872"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{693E145C-E650-345F-689D-D8BB55495237}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2813050" y="38100"/>
+          <a:ext cx="65" cy="187872"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr/>
+          <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
@@ -934,177 +851,63 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="514563" cy="187872"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="TextBox 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41FA0C05-AEB8-CC04-D094-F098E4EFCB68}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4883150" y="25400"/>
-              <a:ext cx="514563" cy="187872"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>(</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>𝑱</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t> / </m:t>
-                    </m:r>
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑱</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝒏</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>)</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1200" b="1"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="TextBox 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41FA0C05-AEB8-CC04-D094-F098E4EFCB68}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4883150" y="25400"/>
-              <a:ext cx="514563" cy="187872"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="1" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>(𝑱 / 𝑱_𝒏)</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1200" b="1"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <xdr:ext cx="65" cy="187872"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41FA0C05-AEB8-CC04-D094-F098E4EFCB68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6026150" y="25400"/>
+          <a:ext cx="65" cy="187872"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr/>
+          <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:colOff>755650</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="303416" cy="193130"/>
+    <xdr:ext cx="195053" cy="187872"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
@@ -1120,8 +923,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5962650" y="38100"/>
-              <a:ext cx="303416" cy="193130"/>
+              <a:off x="7499350" y="38100"/>
+              <a:ext cx="195053" cy="187872"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1148,6 +951,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1178,20 +982,6 @@
                           </a:rPr>
                           <m:t>𝜺</m:t>
                         </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>,</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑵</m:t>
-                        </m:r>
                       </m:sub>
                     </m:sSub>
                   </m:oMath>
@@ -1216,8 +1006,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5962650" y="38100"/>
-              <a:ext cx="303416" cy="193130"/>
+              <a:off x="7499350" y="38100"/>
+              <a:ext cx="195053" cy="187872"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1244,18 +1034,19 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1200" b="1" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑻_(</a:t>
+                <a:t>𝑻_</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1200" b="1" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝜺,𝑵)</a:t>
+                <a:t>𝜺</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1200" b="1"/>
             </a:p>
@@ -1268,9 +1059,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>990600</xdr:colOff>
+      <xdr:colOff>596900</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="195053" cy="187872"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1288,7 +1079,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7518400" y="25400"/>
+              <a:off x="7950200" y="38100"/>
               <a:ext cx="195053" cy="187872"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1316,6 +1107,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1370,7 +1162,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7518400" y="25400"/>
+              <a:off x="7950200" y="38100"/>
               <a:ext cx="195053" cy="187872"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1398,6 +1190,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1200" b="1" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -1412,223 +1205,6 @@
                 <a:t>𝜺</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1200" b="1"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="734688" cy="193130"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="11" name="TextBox 10">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1729EE5-9D16-2E4A-96A9-8B135296AB01}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="8470900" y="38100"/>
-              <a:ext cx="734688" cy="193130"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a14:m>
-                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:sSub>
-                    <m:sSubPr>
-                      <m:ctrlPr>
-                        <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                      </m:ctrlPr>
-                    </m:sSubPr>
-                    <m:e>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>(</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑻</m:t>
-                      </m:r>
-                    </m:e>
-                    <m:sub>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝜺</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>,</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑵</m:t>
-                      </m:r>
-                    </m:sub>
-                  </m:sSub>
-                  <m:r>
-                    <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                    </a:rPr>
-                    <m:t> / </m:t>
-                  </m:r>
-                  <m:sSub>
-                    <m:sSubPr>
-                      <m:ctrlPr>
-                        <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                      </m:ctrlPr>
-                    </m:sSubPr>
-                    <m:e>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑻</m:t>
-                      </m:r>
-                    </m:e>
-                    <m:sub>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝜺</m:t>
-                      </m:r>
-                    </m:sub>
-                  </m:sSub>
-                  <m:r>
-                    <a:rPr lang="en-US" sz="1200" b="1" i="1">
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                    </a:rPr>
-                    <m:t>)</m:t>
-                  </m:r>
-                </m:oMath>
-              </a14:m>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="1"/>
-                <a:t> </a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="11" name="TextBox 10">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1729EE5-9D16-2E4A-96A9-8B135296AB01}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="8470900" y="38100"/>
-              <a:ext cx="734688" cy="193130"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="1" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>〖(𝑻〗_(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="1" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝜺,𝑵)  / 𝑻_𝜺)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="1"/>
-                <a:t> </a:t>
-              </a:r>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -1936,18 +1512,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77EA6114-6834-9F42-81C0-5D3C256F4CB2}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A29"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" customWidth="1"/>
-    <col min="8" max="8" width="26.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" customWidth="1"/>
     <col min="9" max="9" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1955,47 +1532,52 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4">
-        <v>63.16</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4">
-        <v>66.67</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="4">
+        <v>28.19</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -2004,52 +1586,48 @@
       <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="9">
-        <v>0.51600000000000001</v>
-      </c>
+      <c r="D3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="8">
+        <v>16.02</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8">
+        <v>71.349999999999994</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="4">
-        <v>236.41</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="G4" s="4" t="s">
+        <v>59.84</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="5">
-        <v>4.7100000000000003E-2</v>
+      <c r="F4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="4">
+        <v>77.73</v>
+      </c>
+      <c r="H4" s="4">
+        <v>35.57</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -2058,52 +1636,48 @@
       <c r="C5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="8">
-        <v>109.95</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="D5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="8">
+        <v>20.81</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="4">
-        <v>87.08</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="4">
-        <v>4.3700000000000003E-2</v>
+        <v>34.880000000000003</v>
+      </c>
+      <c r="E6" s="4">
+        <v>16.71</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="G6" s="4">
-        <v>83.11</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0.12</v>
+        <v>64.06</v>
+      </c>
+      <c r="H6" s="4">
+        <v>31.95</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -2112,52 +1686,48 @@
       <c r="C7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="9">
-        <v>9.1499999999999998E-2</v>
-      </c>
+      <c r="D7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3">
         <v>21</v>
-      </c>
-      <c r="B8" s="3">
-        <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="4">
-        <v>70.61</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>30</v>
+        <v>17.86</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5.71</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="G8" s="4">
+        <v>53.77</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -2166,52 +1736,48 @@
       <c r="C9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0.22900000000000001</v>
-      </c>
-      <c r="G9" s="8">
-        <v>75.72</v>
-      </c>
-      <c r="H9" s="8" t="s">
+      <c r="D9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="9">
-        <v>0.378</v>
-      </c>
+      <c r="H9" s="8">
+        <v>31.69</v>
+      </c>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="4">
-        <v>201.86</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="4">
-        <v>4.4999999999999997E-3</v>
+        <v>28.28</v>
+      </c>
+      <c r="E10" s="4">
+        <v>5.8</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="G10" s="4">
-        <v>107.05</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" s="5">
-        <v>5.7500000000000002E-2</v>
+        <v>59.79</v>
+      </c>
+      <c r="H10" s="4">
+        <v>51</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -2220,52 +1786,48 @@
       <c r="C11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>52</v>
-      </c>
+      <c r="D11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="4">
-        <v>77.28</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="4">
-        <v>5.1700000000000003E-2</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>49</v>
+        <v>81.86</v>
+      </c>
+      <c r="E12" s="4">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="4">
+        <v>6.32</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -2274,24 +1836,220 @@
       <c r="C13" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8">
+        <v>83.69</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3">
+        <v>18</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>103.53</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="3">
+        <v>91.01</v>
+      </c>
+      <c r="H14" s="3">
+        <v>37.01</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="7">
+        <v>57.47</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>11</v>
+      </c>
+      <c r="B16" s="3">
+        <v>8</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>175.32</v>
+      </c>
+      <c r="E16" s="3">
+        <v>133.59</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7">
+        <v>111.38</v>
+      </c>
+      <c r="H17" s="7">
+        <v>20.8</v>
+      </c>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3">
+        <v>16</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>187.04</v>
+      </c>
+      <c r="E18" s="3">
+        <v>246.16</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="3">
+        <v>110.36</v>
+      </c>
+      <c r="H18" s="3">
+        <v>21.88</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="8" t="s">
+      <c r="H19" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>22</v>
+      </c>
+      <c r="B20" s="3">
+        <v>17</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>118.95</v>
+      </c>
+      <c r="E20" s="3">
+        <v>64.48</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="3">
+        <v>98.67</v>
+      </c>
+      <c r="H20" s="3">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="8">
-        <v>71.69</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I13" s="9">
-        <v>0.14599999999999999</v>
-      </c>
+      <c r="H21" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>